<commit_message>
Added trial 22 and fixed 18
</commit_message>
<xml_diff>
--- a/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Analysis/Original-Runs_no-constants_summary.xlsx
+++ b/data/Fall2024/Network Motif Comparison - 3 gene, 4 node networks/Analysis/Original-Runs_no-constants_summary.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdahlqui\Desktop\ISMB 2025\21 original runs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B3B987-4D48-41D1-830E-DE1EBF94011C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="845" firstSheet="6" activeTab="21" xr2:uid="{61DF7949-D53D-4105-9735-EE06691314FF}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="845"/>
   </bookViews>
   <sheets>
     <sheet name="No Constants" sheetId="1" r:id="rId1"/>
@@ -35,29 +29,14 @@
     <sheet name="19" sheetId="6" r:id="rId20"/>
     <sheet name="20" sheetId="5" r:id="rId21"/>
     <sheet name="21" sheetId="4" r:id="rId22"/>
+    <sheet name="22" sheetId="26" r:id="rId23"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="10">
   <si>
     <t>Trial</t>
   </si>
@@ -85,12 +64,15 @@
   <si>
     <t>re-ran on office desktop</t>
   </si>
+  <si>
+    <t>edited with data from lab computer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,24 +133,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{70519227-5B63-4686-ADE9-D4CF5CB72DF2}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{6D324F20-C91C-4E45-A4F0-8B5D47920066}"/>
-    <cellStyle name="Normal 4" xfId="1" xr:uid="{530E491E-9E52-4105-A481-D94D8643FA3F}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3 2" xfId="4"/>
+    <cellStyle name="Normal 4" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -176,15 +162,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -223,6 +206,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -231,26 +215,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -329,13 +293,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>11</c:v>
@@ -347,10 +311,10 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -401,13 +365,13 @@
                   <c:v>4.1162418001501893</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.2770266514948387</c:v>
+                  <c:v>4.4742410164453847</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.4742410164453847</c:v>
+                  <c:v>4.5806138981294575</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.5806138981294575</c:v>
+                  <c:v>4.9844587765954298</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>5.2996438589642807</c:v>
@@ -419,15 +383,15 @@
                   <c:v>6.8499549880454111</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12.418329134638627</c:v>
+                  <c:v>8.8409890549749708</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>26.960192353119982</c:v>
+                  <c:v>12.418329134638627</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3AE6-4C22-9488-42930035D488}"/>
             </c:ext>
@@ -443,11 +407,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1279891743"/>
-        <c:axId val="1279897503"/>
+        <c:axId val="112662528"/>
+        <c:axId val="112593152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1279891743"/>
+        <c:axId val="112662528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,7 +454,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1279897503"/>
+        <c:crossAx val="112593152"/>
         <c:crossesAt val="1.0000000000000007E-13"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -498,7 +462,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1279897503"/>
+        <c:axId val="112593152"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -552,7 +516,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1279891743"/>
+        <c:crossAx val="112662528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -566,14 +530,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1171,7 +1135,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F86DA50-4012-DB17-F88E-613B20E279DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6F86DA50-4012-DB17-F88E-613B20E279DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1501,27 +1465,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7478D67-BA7D-48FA-92AF-8000621A116E}">
-  <dimension ref="A1:E24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1535,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -1550,7 +1514,7 @@
         <v>26.960192353119982</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>19</v>
       </c>
@@ -1565,7 +1529,7 @@
         <v>5.9285567017171177</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>9</v>
       </c>
@@ -1580,7 +1544,7 @@
         <v>1.5532058220735163</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>15</v>
       </c>
@@ -1595,7 +1559,7 @@
         <v>4.5806138981294575</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>13</v>
       </c>
@@ -1610,7 +1574,7 @@
         <v>4.1162418001501893</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -1625,7 +1589,7 @@
         <v>2.5158177438627733</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>20</v>
       </c>
@@ -1640,7 +1604,7 @@
         <v>0.60187746430833444</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>12</v>
       </c>
@@ -1655,7 +1619,7 @@
         <v>2.2486088556715709</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -1670,7 +1634,7 @@
         <v>6.5284122499237152E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1685,7 +1649,7 @@
         <v>2.0856817647377221E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -1700,7 +1664,7 @@
         <v>5.2996438589642807</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>21</v>
       </c>
@@ -1715,7 +1679,7 @@
         <v>1.1137561179436419</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -1730,13 +1694,13 @@
         <v>0.27386723817829484</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1">
-        <f>'18'!B16</f>
-        <v>4.2770266514948387</v>
+        <f>'17'!B16</f>
+        <v>4.4742410164453847</v>
       </c>
       <c r="D15">
         <v>14</v>
@@ -1745,13 +1709,13 @@
         <v>6.8499549880454111</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1">
-        <f>'17'!B16</f>
-        <v>4.4742410164453847</v>
+        <f>'4'!B16</f>
+        <v>4.5806138981294575</v>
       </c>
       <c r="D16">
         <v>15</v>
@@ -1760,13 +1724,13 @@
         <v>7.977497771292312E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1">
-        <f>'4'!B16</f>
-        <v>4.5806138981294575</v>
+        <f>'22'!B16</f>
+        <v>4.9844587765954298</v>
       </c>
       <c r="D17">
         <v>16</v>
@@ -1775,7 +1739,7 @@
         <v>12.418329134638627</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>11</v>
       </c>
@@ -1790,7 +1754,7 @@
         <v>4.4742410164453847</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -1802,10 +1766,10 @@
         <v>18</v>
       </c>
       <c r="E19">
-        <v>4.2770266514948387</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8.8409890549749708</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>14</v>
       </c>
@@ -1820,57 +1784,72 @@
         <v>2.1391359444392161E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1">
+        <f>'18'!B16</f>
+        <v>8.8409890549749708</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>0.64156040155411242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
         <v>16</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="1">
         <f>'16'!B16</f>
         <v>12.418329134638627</v>
       </c>
-      <c r="D21">
-        <v>20</v>
-      </c>
-      <c r="E21">
-        <v>0.64156040155411242</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22">
+        <v>3.8275664659826956</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1">
         <v>1</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B23" s="1">
         <f>'1'!B16</f>
         <v>26.960192353119982</v>
       </c>
-      <c r="D22">
-        <v>21</v>
-      </c>
-      <c r="E22">
-        <v>3.8275664659826956</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <v>4.9844587765954298</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15">
+      <c r="D24" t="s">
         <v>2</v>
       </c>
-      <c r="E23">
-        <f>AVERAGE(E2:E22)</f>
-        <v>4.1842079899801989</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+      <c r="E24">
+        <f>AVERAGE(E2:E23)</f>
+        <v>4.4280358622572615</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15">
+      <c r="D25" t="s">
         <v>3</v>
       </c>
-      <c r="E24">
-        <f>SUM(E2:E22)</f>
-        <v>87.868367789584184</v>
+      <c r="E25">
+        <f>SUM(E2:E23)</f>
+        <v>97.416788969659748</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B24">
-    <sortCondition ref="B2:B24"/>
+  <sortState ref="A2:B23">
+    <sortCondition ref="B2:B23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1878,16 +1857,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83615C64-E794-4FBF-9071-AD2A44D1D0A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1901,7 +1880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1915,7 +1894,7 @@
         <v>0.89432642580621535</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1929,7 +1908,7 @@
         <v>1.9110787927100354</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1943,7 +1922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1957,7 +1936,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1971,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1985,7 +1964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1999,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -2013,7 +1992,7 @@
         <v>1.1166904282889309E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2027,7 +2006,7 @@
         <v>7.9069811059048461E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -2041,7 +2020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>6.5284122499237152E-2</v>
@@ -2053,16 +2032,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40157B9F-6434-4685-B5EC-1BE86917077B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2076,7 +2055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2090,7 +2069,7 @@
         <v>0.97480512301039324</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2104,7 +2083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2118,7 +2097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2132,7 +2111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2146,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2160,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2174,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -2188,7 +2167,7 @@
         <v>6.3478182652141636E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>9.4777225356157714E-3</v>
@@ -2202,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>7.2846358830500916E-3</v>
@@ -2216,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>2.0856817647377221E-2</v>
@@ -2228,16 +2207,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA995C32-351D-49BE-93C9-576C97468297}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2251,7 +2230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2265,7 +2244,7 @@
         <v>-1.7175519509747377</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2279,7 +2258,7 @@
         <v>-0.13324725174224825</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2293,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2307,7 +2286,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2321,7 +2300,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2335,7 +2314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2349,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0.23389257029170427</v>
@@ -2363,7 +2342,7 @@
         <v>0.51488080234765232</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2377,7 +2356,7 @@
         <v>4.5507438370658555</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2391,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>5.2996438589642807</v>
@@ -2403,16 +2382,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EF0B3D-B400-4975-8CA7-B989EBF30B53}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2426,7 +2405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2440,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2454,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2468,7 +2447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2482,7 +2461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2496,7 +2475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2510,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2524,7 +2503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -2538,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>8.8560944580185638E-2</v>
@@ -2552,7 +2531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>1.025150528137976</v>
@@ -2566,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.1137561179436419</v>
@@ -2578,16 +2557,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8DD21A-91B9-413D-87A7-237727AE6C19}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2601,7 +2580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2615,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2629,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2643,7 +2622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2657,7 +2636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2671,7 +2650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2685,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2699,7 +2678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>3.5055966717856532E-2</v>
@@ -2713,7 +2692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2727,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>2.329951089025865E-2</v>
@@ -2741,7 +2720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>0.27386723817829484</v>
@@ -2753,16 +2732,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142147BB-8850-42AC-BF7C-800B472E78BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2776,7 +2755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2790,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2804,7 +2783,7 @@
         <v>0.77988013174278348</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2818,7 +2797,7 @@
         <v>-0.55811345697717396</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2832,7 +2811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2846,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2860,7 +2839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2874,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>2.4511716013514193E-2</v>
@@ -2888,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -2902,7 +2881,7 @@
         <v>1.4886924929160075</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>2.9090332343025298</v>
@@ -2916,7 +2895,7 @@
         <v>2.4277175448133597</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>6.8499549880454111</v>
@@ -2928,16 +2907,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E82B8F-29E1-4315-852A-14C5AE3CB1A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2951,7 +2930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2965,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2979,7 +2958,7 @@
         <v>1.8941475915385062</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2993,7 +2972,7 @@
         <v>0.90461466440325833</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3007,7 +2986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3021,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3035,7 +3014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3049,7 +3028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3063,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3077,7 +3056,7 @@
         <v>1.1204732377098924E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3091,7 +3070,7 @@
         <v>9.0983622469030332E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>7.977497771292312E-2</v>
@@ -3103,16 +3082,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134DEB53-E5AB-4274-AFB9-D4C08DD6EBEC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3126,7 +3105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3140,7 +3119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3154,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3168,7 +3147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3182,7 +3161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3196,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3210,7 +3189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3224,7 +3203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3238,7 +3217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3252,7 +3231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>8.0381255880144966</v>
@@ -3266,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>12.418329134638627</v>
@@ -3278,16 +3257,16 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F142013-565D-4117-8E1E-C10958E38EE8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3301,7 +3280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3315,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3329,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3343,7 +3322,7 @@
         <v>3.7528717419614527E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3357,7 +3336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3371,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3385,7 +3364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3399,7 +3378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>5.7817854213474497E-2</v>
@@ -3413,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>2.0192789209237123</v>
@@ -3427,7 +3406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>1.470793271516265</v>
@@ -3441,7 +3420,7 @@
         <v>0.92635096979193232</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.4742410164453847</v>
@@ -3453,16 +3432,16 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01013357-7328-4AD5-90E3-3258776CEF5B}">
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D10"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3476,7 +3455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3490,7 +3469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3498,27 +3477,27 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>-1.0887095382589211</v>
+        <v>-0.86394195021244968</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-1.3564270702683929</v>
+        <v>-0.12491009675497475</v>
       </c>
       <c r="C4">
-        <v>0.34141733086855014</v>
+        <v>0.13600552443760247</v>
       </c>
       <c r="D4">
-        <v>-5.0749581532250586E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-0.35352861509626182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3532,7 +3511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3546,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3560,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3574,7 +3553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3588,46 +3567,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>7.8693821781109941E-3</v>
+        <v>1.851179291199152E-2</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15">
       <c r="B14">
         <f t="shared" si="1"/>
-        <v>0.41418611588332405</v>
+        <v>3.515962145251438</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>2.7508964703432044</v>
+        <v>3.4744754049271376</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>1.1040746830901995</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.8320397118844043</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
-        <v>4.2770266514948387</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8.8409890549749708</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15">
       <c r="A19" s="4">
         <v>45846</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="4">
+        <v>45868</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -3636,16 +3623,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B97CF0-99B2-4337-A953-1577F71FE002}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3659,7 +3646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3673,7 +3660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3687,7 +3674,7 @@
         <v>-1.1934713483558728</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3701,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3715,7 +3702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3729,7 +3716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3743,7 +3730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3757,7 +3744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -3771,7 +3758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0.30439781706407848</v>
@@ -3785,7 +3772,7 @@
         <v>4.8113165560581308</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>4.46538461318631</v>
@@ -3799,7 +3786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>26.960192353119982</v>
@@ -3811,16 +3798,16 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76EDBDA-A255-485C-A114-9E4EBC1235F8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3834,7 +3821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3848,7 +3835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3862,7 +3849,7 @@
         <v>1.8844665915805057</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3876,7 +3863,7 @@
         <v>0.96237881530936553</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -3890,7 +3877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -3904,7 +3891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3918,7 +3905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3932,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>6.599065456803067E-3</v>
@@ -3946,7 +3933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -3960,7 +3947,7 @@
         <v>1.3347968461025685E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3974,7 +3961,7 @@
         <v>1.4153535375268293E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>2.1391359444392161E-2</v>
@@ -3986,16 +3973,16 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300E425B-5620-4431-B514-B1BBE2549DEE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4009,7 +3996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4023,7 +4010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4037,7 +4024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4051,7 +4038,7 @@
         <v>0.3672990334850082</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4065,7 +4052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4079,7 +4066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4093,7 +4080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4107,7 +4094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4121,7 +4108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>1.4283999131475694E-3</v>
@@ -4135,7 +4122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4149,7 +4136,7 @@
         <v>0.40031051302900483</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>0.64156040155411242</v>
@@ -4161,16 +4148,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F7287-090A-46B7-BA3C-27A59C785353}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4184,7 +4171,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4198,7 +4185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4212,7 +4199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4226,7 +4213,7 @@
         <v>0.92915440393141491</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4240,7 +4227,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4254,7 +4241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4268,7 +4255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4282,7 +4269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4296,7 +4283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>1.0563570498374768</v>
@@ -4310,7 +4297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>2.7661358697887684</v>
@@ -4324,10 +4311,185 @@
         <v>5.0190984823131196E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>3.8275664659826956</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15">
+      <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5">
+        <v>-2.1720989932914896</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>-2.0023826763422901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.27893139186716043</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.19466783531660359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6">
+        <v>-1</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12">
+        <f>(B8-B2)^2</f>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:D12" si="0">(C8-C2)^2</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15">
+      <c r="B13">
+        <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
+        <v>1.3738160500749232</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>5.6771465521087282E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15">
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>2.9620771539003092</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>0.64855989547364512</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15">
+      <c r="B16" s="2">
+        <f>SUM(B12:D14)</f>
+        <v>4.9844587765954298</v>
       </c>
     </row>
   </sheetData>
@@ -4336,16 +4498,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0089BC1C-C5EA-49A9-99C3-DFC372691FF0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4359,7 +4521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4373,7 +4535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4387,7 +4549,7 @@
         <v>-0.33182484957008046</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4401,7 +4563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4415,7 +4577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -4429,7 +4591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4443,7 +4605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4457,7 +4619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4471,7 +4633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>1.6594589504777784</v>
@@ -4485,7 +4647,7 @@
         <v>1.7737574299323673</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -4499,7 +4661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>5.9285567017171177</v>
@@ -4511,16 +4673,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313B83BB-D4F2-401B-BF0B-10D69BB3D6FD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4534,7 +4696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4548,7 +4710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4562,7 +4724,7 @@
         <v>1.0749142632919517</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4576,7 +4738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4590,7 +4752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4604,7 +4766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4618,7 +4780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4632,7 +4794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0.3208399102785181</v>
@@ -4646,7 +4808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -4660,7 +4822,7 @@
         <v>5.6121468445758651E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>1.5298837410739096E-3</v>
@@ -4674,7 +4836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>1.5532058220735163</v>
@@ -4686,16 +4848,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3D4390-3995-460B-ABEF-C18D95517F47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4709,7 +4871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4723,7 +4885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4737,7 +4899,7 @@
         <v>1.4105857766672745</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4751,7 +4913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4765,7 +4927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4779,7 +4941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4793,7 +4955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4807,7 +4969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -4821,7 +4983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -4835,7 +4997,7 @@
         <v>0.168580680001469</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -4849,7 +5011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.5806138981294575</v>
@@ -4861,16 +5023,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB9E05B-3793-41C3-B94B-40F5229BD806}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4884,7 +5046,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4898,7 +5060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4912,7 +5074,7 @@
         <v>0.52988859423036627</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4926,7 +5088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -4940,7 +5102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -4954,7 +5116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -4968,7 +5130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -4982,7 +5144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>3.076316093291815</v>
@@ -4996,7 +5158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5010,7 +5172,7 @@
         <v>0.22100473383470121</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5024,7 +5186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>4.1162418001501893</v>
@@ -5036,16 +5198,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6FF64C-47D1-4ACB-8BCD-8DB8DA890DE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5059,7 +5221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5073,7 +5235,7 @@
         <v>-0.9522160640197086</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5087,7 +5249,7 @@
         <v>0.92901819187744683</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5101,7 +5263,7 @@
         <v>-1.7246037824720879</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5115,7 +5277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5129,7 +5291,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5143,7 +5305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5157,7 +5319,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -5171,7 +5333,7 @@
         <v>2.2833045377685874E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5185,7 +5347,7 @@
         <v>1.1470020333294531</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5199,7 +5361,7 @@
         <v>7.5843076628681075E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>2.5158177438627733</v>
@@ -5211,16 +5373,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C51A42-0714-4274-9CCE-FD3E5D511EAB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -5246,7 +5408,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -5272,7 +5434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -5298,7 +5460,7 @@
         <v>0.45344311379413876</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -5324,7 +5486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -5350,7 +5512,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -5376,7 +5538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -5402,7 +5564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -5428,7 +5590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>1.1145103613289806E-3</v>
@@ -5454,7 +5616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="2">(B9-B3)^2</f>
         <v>0.28916923042100023</v>
@@ -5480,7 +5642,7 @@
         <v>0.29872442985904668</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>0</v>
@@ -5506,7 +5668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>0.60187746430833444</v>
@@ -5522,16 +5684,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{743B6CCE-E37A-4B9D-B598-F019BFB3039F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -5545,7 +5707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5559,7 +5721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5573,7 +5735,7 @@
         <v>1.0734930225760295</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5587,7 +5749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -5601,7 +5763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -5615,7 +5777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -5629,7 +5791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -5643,7 +5805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12">
         <f>(B8-B2)^2</f>
         <v>0</v>
@@ -5657,7 +5819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13">
         <f t="shared" ref="B13:D14" si="1">(B9-B3)^2</f>
         <v>0</v>
@@ -5671,7 +5833,7 @@
         <v>5.4012243673607846E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14">
         <f>(B10-B4)^2</f>
         <v>2.027326322907663E-4</v>
@@ -5685,7 +5847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="2">
         <f>SUM(B12:D14)</f>
         <v>2.2486088556715709</v>
@@ -5697,23 +5859,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="070f1269-45c1-4463-99ba-5dc4e57c7dff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008DB5B7ED115EF04980BBFAFC51672553" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="43a679fe5cbd3b1dc01cea5b3bb6a16a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="070f1269-45c1-4463-99ba-5dc4e57c7dff" xmlns:ns4="7bf50b4b-6300-445a-aea1-306a2291592c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0963d0390b393dc53bf13ff5a8315f4" ns3:_="" ns4:_="">
     <xsd:import namespace="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
@@ -5908,25 +6053,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE723E-1688-4D1F-8FE6-FDF46584855C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="070f1269-45c1-4463-99ba-5dc4e57c7dff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAD4690-B959-480E-AC59-DDDE87F8E768}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02EB7017-44D4-47C1-BB45-296DD07AFBB9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5943,4 +6087,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAD4690-B959-480E-AC59-DDDE87F8E768}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="070f1269-45c1-4463-99ba-5dc4e57c7dff"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2EE723E-1688-4D1F-8FE6-FDF46584855C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>